<commit_message>
chore: Add Richard Feynman AI Chat functionality steamlit file
</commit_message>
<xml_diff>
--- a/model_comparison_summary.xlsx
+++ b/model_comparison_summary.xlsx
@@ -452,27 +452,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.71</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>gpt-4-0125-preview</t>
+          <t>gpt-4o-mini</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>ft:gpt-4o-mini-2024-07-18:redhorse:500-mathproblem:9q7KKy7G</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>